<commit_message>
Adds ?j2sheadless and ?j2sprofile; allows getApplet(Info); allows Info.name;
removes all references in Java of getting
System.getProperty("java.awt.headless")
</commit_message>
<xml_diff>
--- a/sources/net.sf.j2s.java.core/dev/j2sflags.xlsx
+++ b/sources/net.sf.j2s.java.core/dev/j2sflags.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t>j2sdebugclip</t>
   </si>
@@ -63,15 +63,6 @@
     <t>j2sverbose</t>
   </si>
   <si>
-    <t>same as j2snocore?</t>
-  </si>
-  <si>
-    <t>same as j2snozcore?</t>
-  </si>
-  <si>
-    <t>preferred language; application should check</t>
-  </si>
-  <si>
     <t>strict mode -- experimental</t>
   </si>
   <si>
@@ -126,12 +117,6 @@
     <t>j2sargs=a|b|c</t>
   </si>
   <si>
-    <t>arguments to be passed on to application.main(); use "|" to separate arguments.</t>
-  </si>
-  <si>
-    <t>j2slang=EN_us</t>
-  </si>
-  <si>
     <t>report mouse events other than mousemove</t>
   </si>
   <si>
@@ -144,9 +129,6 @@
     <t>use the uncompressed j2s/core/xxxcore.js files, not the compressed core.z.js files</t>
   </si>
   <si>
-    <t>track object creation; use J2S.getProfile() when you want a report, after that J2S.getProfile() or J2S.getProfile(nsec) to restart profiling anytime.</t>
-  </si>
-  <si>
     <t>use new Function() instead of eval(); breaks debugging, experimental</t>
   </si>
   <si>
@@ -169,6 +151,30 @@
   </si>
   <si>
     <t>This is the "source" of site-resources/__j2sflags.htm</t>
+  </si>
+  <si>
+    <t>j2sheadless</t>
+  </si>
+  <si>
+    <t>run headlessly (must be a main()-based application or library without Swing or AWT)</t>
+  </si>
+  <si>
+    <t>j2slang=en_US</t>
+  </si>
+  <si>
+    <t>default language for java.util.Locale (overrides Info.language)</t>
+  </si>
+  <si>
+    <t>track object creation; use J2S.getProfile() when you want a report; J2S.getProfile() or J2S.getProfile(nsec) to restart profiling anytime.</t>
+  </si>
+  <si>
+    <t>arguments to be passed on to application.main(); use "|" to separate arguments. Overrides Info.args, which should be an array of strings, if present</t>
+  </si>
+  <si>
+    <t>deprecated; see j2snocore</t>
+  </si>
+  <si>
+    <t>deprecated; see j2snozcore</t>
   </si>
 </sst>
 </file>
@@ -986,10 +992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -999,21 +1005,21 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1022,10 +1028,10 @@
         <v>&lt;head&gt;&lt;title&gt;URL command line flags for SwingJS&lt;/title&gt;&lt;/head&gt;</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1034,10 +1040,10 @@
         <v>&lt;body&gt;&lt;h3&gt;URL command-line arguments for SwingJS&lt;/h3&gt;</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1046,7 +1052,7 @@
         <v>&lt;br&gt;To enable these flags, simply add them after # or ? on your page.</v>
       </c>
       <c r="F5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1055,7 +1061,7 @@
         <v xml:space="preserve">&lt;br&gt;The test is very simple -- just a case-sensitive string check. </v>
       </c>
       <c r="F6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -1064,7 +1070,7 @@
         <v>&lt;br&gt;Separate them with &amp;amp; For example:</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.35">
@@ -1073,15 +1079,15 @@
         <v>&lt;br&gt;&lt;a href="test_Test_Class.html?j2sverbose&amp;j2snozcore&amp;j2strace=applet"&gt;test_Test_Class.html?j2sverbose&amp;j2snozcore&amp;j2strace=applet&lt;/a&gt;</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -1090,68 +1096,68 @@
         <v>&lt;tr&gt;&lt;th colspan="2"&gt;&lt;/th&gt;&lt;/tr&gt;</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="str">
         <f>"&lt;tr&gt;&lt;td&gt;"&amp;C11&amp;"&lt;/td&gt;&lt;td&gt;"&amp;F11&amp;"&lt;/td&gt;&lt;/tr&gt;"</f>
-        <v>&lt;tr&gt;&lt;td&gt;j2sargs=a|b|c&lt;/td&gt;&lt;td&gt;arguments to be passed on to application.main(); use "|" to separate arguments.&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;j2sargs=a|b|c&lt;/td&gt;&lt;td&gt;arguments to be passed on to application.main(); use "|" to separate arguments. Overrides Info.args, which should be an array of strings, if present&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="str">
-        <f t="shared" ref="A12:A28" si="0">"&lt;tr&gt;&lt;td&gt;"&amp;C12&amp;"&lt;/td&gt;&lt;td&gt;"&amp;F12&amp;"&lt;/td&gt;&lt;/tr&gt;"</f>
+        <f t="shared" ref="A12:A29" si="0">"&lt;tr&gt;&lt;td&gt;"&amp;C12&amp;"&lt;/td&gt;&lt;td&gt;"&amp;F12&amp;"&lt;/td&gt;&lt;/tr&gt;"</f>
         <v>&lt;tr&gt;&lt;td&gt;j2sdebugclip&lt;/td&gt;&lt;td&gt;shows all show/restore and clip operations in JSGraphics2D&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
       <c r="F12" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;j2sdebugcode&lt;/td&gt;&lt;td&gt;same as j2snocore?&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;j2sdebugcode&lt;/td&gt;&lt;td&gt;deprecated; see j2snocore&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="B13" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
         <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>14</v>
+        <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;j2sdebugcore&lt;/td&gt;&lt;td&gt;same as j2snozcore?&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;j2sdebugcore&lt;/td&gt;&lt;td&gt;deprecated; see j2snozcore&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="B14" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C14" t="s">
         <v>2</v>
       </c>
       <c r="F14" t="s">
-        <v>15</v>
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.35">
@@ -1160,13 +1166,13 @@
         <v>&lt;tr&gt;&lt;td&gt;j2sdebugpaint&lt;/td&gt;&lt;td&gt;report repaint manager information&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="B15" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -1175,217 +1181,232 @@
         <v>&lt;tr&gt;&lt;td&gt;j2sevents&lt;/td&gt;&lt;td&gt;report ComponentEvent instances&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="F16" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A17" si="1">"&lt;tr&gt;&lt;td&gt;"&amp;C17&amp;"&lt;/td&gt;&lt;td&gt;"&amp;F17&amp;"&lt;/td&gt;&lt;/tr&gt;"</f>
         <v>&lt;tr&gt;&lt;td&gt;j2sfilter=xxx&lt;/td&gt;&lt;td&gt;remove messages with the specified text from System.out&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="B17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C17" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F17" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;j2slang=EN_us&lt;/td&gt;&lt;td&gt;preferred language; application should check&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;j2sheadless&lt;/td&gt;&lt;td&gt;run headlessly (must be a main()-based application or library without Swing or AWT)&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="B18" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="F18" t="s">
-        <v>16</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;j2smouse&lt;/td&gt;&lt;td&gt;report mouse events other than mousemove&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;j2slang=en_US&lt;/td&gt;&lt;td&gt;default language for java.util.Locale (overrides Info.language)&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="F19" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;j2smousemove&lt;/td&gt;&lt;td&gt;report all mouse events, including mousemove&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;j2smouse&lt;/td&gt;&lt;td&gt;report mouse events other than mousemove&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="F20" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;j2snocore&lt;/td&gt;&lt;td&gt;do not load core files (from j2s/core/)&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;j2smousemove&lt;/td&gt;&lt;td&gt;report all mouse events, including mousemove&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;j2snoeval&lt;/td&gt;&lt;td&gt;use new Function() instead of eval(); breaks debugging, experimental&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;j2snocore&lt;/td&gt;&lt;td&gt;do not load core files (from j2s/core/)&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F22" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;j2snooutput&lt;/td&gt;&lt;td&gt;report only System.err message, not  System.out &lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;j2snoeval&lt;/td&gt;&lt;td&gt;use new Function() instead of eval(); breaks debugging, experimental&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C23" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F23" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;j2snozcore&lt;/td&gt;&lt;td&gt;use the uncompressed j2s/core/xxxcore.js files, not the compressed core.z.js files&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;j2snooutput&lt;/td&gt;&lt;td&gt;report only System.err message, not  System.out &lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F24" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;j2sprofile&lt;/td&gt;&lt;td&gt;track object creation; use J2S.getProfile() when you want a report, after that J2S.getProfile() or J2S.getProfile(nsec) to restart profiling anytime.&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;j2snozcore&lt;/td&gt;&lt;td&gt;use the uncompressed j2s/core/xxxcore.js files, not the compressed core.z.js files&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C25" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;j2sstrict&lt;/td&gt;&lt;td&gt;strict mode -- experimental&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;j2sprofile&lt;/td&gt;&lt;td&gt;track object creation; use J2S.getProfile() when you want a report; J2S.getProfile() or J2S.getProfile(nsec) to restart profiling anytime.&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="B26" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F26" t="s">
-        <v>17</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="str">
         <f t="shared" si="0"/>
-        <v>&lt;tr&gt;&lt;td&gt;j2strace=xxx or j2strace="xxx"&lt;/td&gt;&lt;td&gt;throw up an alert in the browser and a debugger statement in the developer whenever the specified text is found in System.out or System.err; if quotes are used, this must be an exact match to the entire output text (particularly useful when the message is something like "0", which otherwise would be next to impossible to find.&lt;/td&gt;&lt;/tr&gt;</v>
+        <v>&lt;tr&gt;&lt;td&gt;j2sstrict&lt;/td&gt;&lt;td&gt;strict mode -- experimental&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C27" t="s">
-        <v>45</v>
+        <v>12</v>
       </c>
       <c r="F27" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="str">
         <f t="shared" si="0"/>
+        <v>&lt;tr&gt;&lt;td&gt;j2strace=xxx or j2strace="xxx"&lt;/td&gt;&lt;td&gt;throw up an alert in the browser and a debugger statement in the developer whenever the specified text is found in System.out or System.err; if quotes are used, this must be an exact match to the entire output text (particularly useful when the message is something like "0", which otherwise would be next to impossible to find.&lt;/td&gt;&lt;/tr&gt;</v>
+      </c>
+      <c r="B28" t="s">
+        <v>20</v>
+      </c>
+      <c r="C28" t="s">
+        <v>39</v>
+      </c>
+      <c r="F28" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29" t="str">
+        <f t="shared" si="0"/>
         <v>&lt;tr&gt;&lt;td&gt;j2sverbose&lt;/td&gt;&lt;td&gt;report all files loaded using AJAX&lt;/td&gt;&lt;/tr&gt;</v>
       </c>
-      <c r="B28" t="s">
-        <v>23</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="B29" t="s">
+        <v>20</v>
+      </c>
+      <c r="C29" t="s">
         <v>13</v>
       </c>
-      <c r="F28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>18</v>
-      </c>
-      <c r="B29" t="s">
-        <v>23</v>
+      <c r="F29" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B31" t="s">
-        <v>23</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>18</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>